<commit_message>
[V&V] Adicionando link de RH na Planilha
Foi adicionado mais 1 link no RAP 7
</commit_message>
<xml_diff>
--- a/Artefatos de Documentação/Processo Aplicado/EveRemind/6-Verificacao e Validacao/PLA-Planilha de Avaliação-VER-VAL.xlsx
+++ b/Artefatos de Documentação/Processo Aplicado/EveRemind/6-Verificacao e Validacao/PLA-Planilha de Avaliação-VER-VAL.xlsx
@@ -15,12 +15,12 @@
     <sheet name="VER" sheetId="36" r:id="rId1"/>
     <sheet name="VAL" sheetId="35" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="77">
   <si>
     <t>Projeto 1</t>
   </si>
@@ -520,6 +520,9 @@
   </si>
   <si>
     <t>RT - Resultados de Teste &gt; Seção 3.3</t>
+  </si>
+  <si>
+    <t>RH - Recursos Humanos &gt; Seção de Treinamentos</t>
   </si>
 </sst>
 </file>
@@ -979,7 +982,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1205,6 +1208,9 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1619,8 +1625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A88" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E100" sqref="E100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -2832,7 +2838,7 @@
     </row>
     <row r="96" spans="1:8" ht="15">
       <c r="A96" s="73" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B96" s="20"/>
       <c r="C96" s="75" t="s">
@@ -2863,10 +2869,14 @@
       <c r="H97" s="57"/>
     </row>
     <row r="98" spans="1:8">
-      <c r="A98" s="19"/>
+      <c r="A98" s="82" t="s">
+        <v>76</v>
+      </c>
       <c r="B98" s="18"/>
       <c r="C98" s="70"/>
-      <c r="D98" s="70"/>
+      <c r="D98" s="75" t="s">
+        <v>17</v>
+      </c>
       <c r="E98" s="18"/>
       <c r="F98" s="18"/>
       <c r="G98" s="18"/>
@@ -3264,9 +3274,10 @@
     <hyperlink ref="D120" r:id="rId76"/>
     <hyperlink ref="C38" r:id="rId77"/>
     <hyperlink ref="D38" r:id="rId78"/>
+    <hyperlink ref="D98" r:id="rId79"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.49212598499999999" footer="0.49212598499999999"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId79"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId80"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>